<commit_message>
Open API 2.3 ver 스펙문서
</commit_message>
<xml_diff>
--- a/NSMall_EDI_API_Specs_v2.3_20230919.xlsx
+++ b/NSMall_EDI_API_Specs_v2.3_20230919.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\업무관련설계서\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Desktop\업무관련설계서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CEE0EE5-79CE-4EAD-B366-215CC10AEDB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2A42B7-CC4C-43F2-9D13-6340A62C3101}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" tabRatio="893" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" tabRatio="893" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="표지" sheetId="63" r:id="rId1"/>
@@ -11264,10 +11264,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>단품가격수정 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>강석진</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -11350,6 +11346,11 @@
   <si>
     <t>전시매장 그룹 아이디_삭제대상</t>
     <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>단품가격수정 추가
+전시매장수정 삭제기능 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -12176,7 +12177,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -12733,6 +12734,9 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="KAL_문서_표준" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -12789,8 +12793,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1369135" y="7494494"/>
-          <a:ext cx="4493559" cy="997100"/>
+          <a:off x="1373281" y="7382435"/>
+          <a:ext cx="4502523" cy="976593"/>
           <a:chOff x="144" y="718"/>
           <a:chExt cx="472" cy="89"/>
         </a:xfrm>
@@ -18090,7 +18094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A7:H39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -18247,12 +18251,12 @@
     </row>
     <row r="11" spans="1:8" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F11" s="17" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="25.2" x14ac:dyDescent="0.55000000000000004">
       <c r="F12" s="17" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="39" spans="6:6" ht="21" x14ac:dyDescent="0.45">
@@ -23350,7 +23354,7 @@
         <v>25</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
@@ -23451,13 +23455,13 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="102"/>
       <c r="B15" s="31" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="C15" s="34">
         <v>0</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="E15" s="103" t="s">
         <v>49</v>
@@ -23469,19 +23473,19 @@
         <v>224</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="102"/>
       <c r="B16" s="31" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="C16" s="34">
         <v>0</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>28</v>
@@ -23493,7 +23497,7 @@
         <v>224</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
@@ -23895,7 +23899,7 @@
         <v>575</v>
       </c>
       <c r="J11" s="135" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="39.6" x14ac:dyDescent="0.4">
@@ -24009,7 +24013,7 @@
         <v>52</v>
       </c>
       <c r="B17" s="162" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="C17" s="163"/>
       <c r="D17" s="163"/>
@@ -24023,7 +24027,7 @@
         <v>54</v>
       </c>
       <c r="B18" s="162" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="C18" s="168"/>
       <c r="D18" s="168"/>
@@ -25880,7 +25884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A5:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12:J12"/>
     </sheetView>
   </sheetViews>
@@ -25997,11 +26001,11 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D10" s="136" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="E10" s="137"/>
       <c r="F10" s="138" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="G10" s="139"/>
       <c r="H10" s="139"/>
@@ -26023,15 +26027,15 @@
         <v>1426</v>
       </c>
       <c r="E11" s="137"/>
-      <c r="F11" s="138" t="s">
-        <v>1427</v>
+      <c r="F11" s="185" t="s">
+        <v>1441</v>
       </c>
       <c r="G11" s="139"/>
       <c r="H11" s="139"/>
       <c r="I11" s="139"/>
       <c r="J11" s="140"/>
       <c r="K11" s="120" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="L11" s="120" t="s">
         <v>1401</v>
@@ -26248,42 +26252,6 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:J26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:J27"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:J23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:J24"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:J12"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="A5:O5"/>
@@ -26291,6 +26259,42 @@
     <mergeCell ref="F7:J7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:J8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:J24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:J26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:J27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>